<commit_message>
9/15/2024 from PC: 1
</commit_message>
<xml_diff>
--- a/2024/Fall 2024/TFES Lab/Flow Visualization/FlowVisLab_RawDataSheet.xlsx
+++ b/2024/Fall 2024/TFES Lab/Flow Visualization/FlowVisLab_RawDataSheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\babyl\OneDrive\Documents\School\2024\Fall 2024\TFES Lab\Flow Visualization\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brand\Documents\SchoolFiles\2024\Fall 2024\TFES Lab\Flow Visualization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08BCDB6A-3B43-498A-9F75-CD9491442D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3051151-E663-4C04-881C-B14624A16B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43095" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Sheet" sheetId="1" r:id="rId1"/>
@@ -1104,21 +1104,21 @@
   <dimension ref="B1:M32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="24.77734375" customWidth="1"/>
-    <col min="3" max="3" width="31.33203125" customWidth="1"/>
-    <col min="4" max="7" width="20.77734375" customWidth="1"/>
-    <col min="8" max="8" width="8.77734375" customWidth="1"/>
-    <col min="9" max="9" width="14.77734375" customWidth="1"/>
-    <col min="10" max="10" width="10.77734375" customWidth="1"/>
-    <col min="11" max="13" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
+    <col min="3" max="3" width="31.28515625" customWidth="1"/>
+    <col min="4" max="7" width="20.7109375" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" customWidth="1"/>
+    <col min="11" max="13" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="28.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:13" ht="27.75" x14ac:dyDescent="0.2">
       <c r="B1" s="50" t="s">
         <v>1</v>
       </c>
@@ -1131,7 +1131,7 @@
       <c r="I1" s="20"/>
       <c r="J1" s="8"/>
     </row>
-    <row r="2" spans="2:13" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:13" ht="37.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="51" t="s">
         <v>4</v>
       </c>
@@ -1144,7 +1144,7 @@
       <c r="I2" s="21"/>
       <c r="J2" s="10"/>
     </row>
-    <row r="3" spans="2:13" ht="37.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:13" ht="37.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="16" t="s">
         <v>2</v>
       </c>
@@ -1158,7 +1158,7 @@
       </c>
       <c r="G3" s="17"/>
     </row>
-    <row r="4" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
@@ -1169,7 +1169,7 @@
       <c r="I4" s="9"/>
       <c r="J4" s="10"/>
     </row>
-    <row r="5" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
@@ -1180,7 +1180,7 @@
       <c r="I5" s="9"/>
       <c r="J5" s="10"/>
     </row>
-    <row r="6" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="9"/>
       <c r="C6" s="3" t="s">
         <v>5</v>
@@ -1193,7 +1193,7 @@
       <c r="G6" s="9"/>
       <c r="H6" s="10"/>
     </row>
-    <row r="7" spans="2:13" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:13" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="3"/>
@@ -1207,7 +1207,7 @@
       <c r="L7" s="6"/>
       <c r="M7" s="5"/>
     </row>
-    <row r="8" spans="2:13" ht="42" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:13" ht="42" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="31" t="s">
         <v>6</v>
       </c>
@@ -1227,7 +1227,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="2:13" ht="28.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:13" ht="28.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="45" t="s">
         <v>9</v>
       </c>
@@ -1247,7 +1247,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="2:13" ht="28.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:13" ht="28.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="46"/>
       <c r="C10" s="30" t="s">
         <v>20</v>
@@ -1265,7 +1265,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="2:13" ht="28.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:13" ht="28.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="46"/>
       <c r="C11" s="30" t="s">
         <v>21</v>
@@ -1283,7 +1283,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="2:13" ht="28.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:13" ht="28.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="47"/>
       <c r="C12" s="24" t="s">
         <v>22</v>
@@ -1301,7 +1301,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="2:13" ht="28.05" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:13" ht="28.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B13" s="45" t="s">
         <v>12</v>
       </c>
@@ -1321,7 +1321,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="2:13" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:13" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="46"/>
       <c r="C14" s="30" t="s">
         <v>14</v>
@@ -1339,7 +1339,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="2:13" ht="28.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:13" ht="28.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="47"/>
       <c r="C15" s="24" t="s">
         <v>15</v>
@@ -1357,7 +1357,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="2:13" ht="28.05" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:13" ht="28.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B16" s="45" t="s">
         <v>16</v>
       </c>
@@ -1377,7 +1377,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="2:10" ht="28.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:10" ht="28.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" s="47"/>
       <c r="C17" s="24" t="s">
         <v>24</v>
@@ -1395,7 +1395,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="2:10" ht="28.05" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" ht="28.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B18" s="48" t="s">
         <v>39</v>
       </c>
@@ -1415,7 +1415,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="2:10" ht="28.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:10" ht="28.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="49"/>
       <c r="C19" s="24" t="s">
         <v>41</v>
@@ -1433,8 +1433,8 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="2:10" ht="9" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="2:10" ht="52.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" ht="9" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="2:10" ht="52.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D21" s="12"/>
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
@@ -1442,23 +1442,23 @@
       <c r="I21" s="12"/>
       <c r="J21" s="13"/>
     </row>
-    <row r="22" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J27" s="1"/>
     </row>
-    <row r="28" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J28" s="1"/>
     </row>
-    <row r="29" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J29" s="1"/>
     </row>
-    <row r="30" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="B13:B15"/>

</xml_diff>